<commit_message>
Chatbot test content updates
</commit_message>
<xml_diff>
--- a/content/Chatbot Intents.xlsx
+++ b/content/Chatbot Intents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\hau-ai-powered-lms\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1849BDA-651A-4D02-96FA-117083D8C7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494CBEF8-459A-4707-9291-50659B3763BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54BB7CB1-154D-4315-B860-206F774AA722}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>ask.what_is_ml</t>
   </si>
   <si>
-    <t>what is machine learning?;</t>
-  </si>
-  <si>
     <t>Good afternoon, how can I help you?;</t>
   </si>
   <si>
@@ -113,7 +110,10 @@
     <t>I'm John the geek! My job is to help you understand AI and Innovation</t>
   </si>
   <si>
-    <t>hi; hello; how are you doing?; how is it going?</t>
+    <t>hi; hello; how are you doing?; how is it going?; Hi?; Hello?</t>
+  </si>
+  <si>
+    <t>what is machine learning?; what is ML?;</t>
   </si>
 </sst>
 </file>
@@ -468,13 +468,13 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="195.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,7 +494,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -530,7 +530,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -538,43 +538,43 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
react, tensorflow and nlp intents
</commit_message>
<xml_diff>
--- a/content/Chatbot Intents.xlsx
+++ b/content/Chatbot Intents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\hau-ai-powered-lms\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BA8873-AF17-4CA8-B455-26E68EED4B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943BEB70-771C-4FAF-9AD9-5F9C611ACDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54BB7CB1-154D-4315-B860-206F774AA722}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="241">
   <si>
     <t>intent</t>
   </si>
@@ -726,6 +726,36 @@
   </si>
   <si>
     <t>haha; hahaha; lol; :D; ^_^; ROFL; (rofl); HAHAHA; hahaha;</t>
+  </si>
+  <si>
+    <t>ask.what_is_tensorflow</t>
+  </si>
+  <si>
+    <t>what is tensorflow?; describe tensorflow?; tell me something about Tensorflow?; define Tensorflow?; explain tensorflow?;</t>
+  </si>
+  <si>
+    <t>TensorFlow is a free and open-source software library for machine learning and artificial intelligence. It can be used across a range of tasks but has a particular focus on training and inference of deep neural networks. TensorFlow provides a collection of workflows to develop and train models using Python or JavaScript, and to easily deploy in the cloud, on-prem, in the browser, or on-device no matter what language you use. The tf. data API enables you to build complex input pipelines from simple, reusable pieces.</t>
+  </si>
+  <si>
+    <t>ask.what_is_react</t>
+  </si>
+  <si>
+    <t>ask.what_is_nlp</t>
+  </si>
+  <si>
+    <t>A table is an arrangement of information or data, typically in rows and columns, or possibly in a more complex structure. Tables are widely used in communication, research, and data analysis.</t>
+  </si>
+  <si>
+    <t>what is react?; what is react.js; what is React JS?; do you know react js?;</t>
+  </si>
+  <si>
+    <t>what is nlp?; describe NLP?; define NLP; explain NLP; can you explain NLP?;</t>
+  </si>
+  <si>
+    <t>NLP or Natural language processing is a subfield of linguistics, computer science, and artificial intelligence concerned with the interactions between computers and human language, in particular how to program computers to process and analyze large amounts of natural language data.</t>
+  </si>
+  <si>
+    <t>React is a free and open-source front-end JavaScript library for building user interfaces based on UI components. It is maintained by Meta and a community of individual developers and companies. React can be used as a base in the development of single-page or mobile applications.</t>
   </si>
 </sst>
 </file>
@@ -1089,16 +1119,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4A59E91-381A-4288-8AAA-0174747CCACE}">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="89.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="113.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1971,8 +2001,52 @@
         <v>228</v>
       </c>
     </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>231</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C80" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>234</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C81" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>235</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C82" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>55</v>
+      </c>
+      <c r="B83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83" t="s">
+        <v>236</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>